<commit_message>
Fix calculated fields refresh bug, add more complex test.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>Transaction</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Sum of CalculatedField2</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>Total Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>Total Sum of CalculatedField</t>
+  </si>
+  <si>
+    <t>Chicago Total</t>
+  </si>
+  <si>
+    <t>Nashville Total</t>
   </si>
 </sst>
 </file>
@@ -242,13 +260,17 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Units Sold" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="6"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Total" numFmtId="8">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="1194"/>
     </cacheField>
     <cacheField name="CalculatedField" numFmtId="0" formula="'Wholesale Price'*'Units Sold'" databaseField="0"/>
-    <cacheField name="CalculatedField2" numFmtId="0" formula="CalculatedField /'Wholesale Price'" databaseField="0"/>
+    <cacheField name="CalculatedField2" numFmtId="0" formula="CalculatedField/'Wholesale Price'" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -266,7 +288,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="1"/>
+    <x v="0"/>
     <n v="415.75"/>
   </r>
   <r>
@@ -275,7 +297,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="1"/>
+    <x v="0"/>
     <n v="99"/>
   </r>
   <r>
@@ -284,7 +306,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="1"/>
+    <x v="0"/>
     <n v="24.99"/>
   </r>
   <r>
@@ -293,7 +315,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="1"/>
     <n v="831.5"/>
   </r>
   <r>
@@ -302,7 +324,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="6"/>
+    <x v="2"/>
     <n v="1194"/>
   </r>
   <r>
@@ -311,7 +333,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="1"/>
     <n v="831.5"/>
   </r>
   <r>
@@ -320,14 +342,126 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2"/>
+    <x v="1"/>
     <n v="831.5"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G4:L14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="5" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of CalculatedField" fld="7" baseField="0" baseItem="0" numFmtId="8"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B18:D27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -412,8 +546,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -982,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+  <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,14 +1128,38 @@
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="17" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" customWidth="1"/>
+    <col min="24" max="24" width="35" customWidth="1"/>
+    <col min="25" max="25" width="34.28515625" customWidth="1"/>
+    <col min="26" max="26" width="27.42578125" customWidth="1"/>
+    <col min="27" max="27" width="26.7109375" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="22.42578125" customWidth="1"/>
+    <col min="31" max="31" width="35" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.28515625" customWidth="1"/>
+    <col min="34" max="34" width="27.42578125" customWidth="1"/>
+    <col min="35" max="35" width="26.7109375" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" customWidth="1"/>
+    <col min="37" max="37" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1011,8 +1169,14 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1023,7 +1187,7 @@
         <v>11641</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1033,8 +1197,11 @@
       <c r="D4" s="3">
         <v>831.5</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1044,8 +1211,23 @@
       <c r="D5" s="3">
         <v>3326</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1055,8 +1237,17 @@
       <c r="D6" s="3">
         <v>415.75</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
@@ -1066,8 +1257,16 @@
       <c r="D7" s="3">
         <v>24.99</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1077,8 +1276,26 @@
       <c r="D8" s="3">
         <v>24.99</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="I8" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="J8" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="K8" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="L8" s="3">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1088,8 +1305,22 @@
       <c r="D9" s="3">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="K9" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="L9" s="3">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1099,8 +1330,16 @@
       <c r="D10" s="3">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1110,8 +1349,26 @@
       <c r="D11" s="3">
         <v>1194</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="K11" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="L11" s="7">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
@@ -1121,8 +1378,26 @@
       <c r="D12" s="3">
         <v>1194</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="K12" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="L12" s="7">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1131,6 +1406,44 @@
       </c>
       <c r="D13" s="3">
         <v>29789.85</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="I13" s="3">
+        <v>415.75</v>
+      </c>
+      <c r="J13" s="3">
+        <v>831.5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>831.5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1247.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="I14" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="J14" s="7">
+        <v>3326</v>
+      </c>
+      <c r="K14" s="7">
+        <v>3326</v>
+      </c>
+      <c r="L14" s="7">
+        <v>7483.5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix exception caused by attempting to sort items in a calculated field. Update test workbook to reproduce this issue.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ems\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -468,13 +468,13 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
+        <item x="2"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
       <items count="5">
         <item x="0"/>
         <item x="2"/>
@@ -482,6 +482,15 @@
         <item x="3"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField numFmtId="8" showAll="0"/>
     <pivotField showAll="0"/>
@@ -500,23 +509,23 @@
     <i r="1">
       <x/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
     <i r="1">
+      <x/>
+    </i>
+    <i>
       <x v="2"/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
-    <i>
+    <i r="1">
       <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1118,15 +1127,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
@@ -1459,13 +1468,13 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7">
-        <v>6236.25</v>
+        <v>1322.22</v>
       </c>
       <c r="D19" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -1473,73 +1482,73 @@
         <v>9</v>
       </c>
       <c r="C20" s="7">
+        <v>831.5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7">
+        <v>24.99</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7">
         <v>6236.25</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D22" s="7">
         <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7">
-        <v>2086</v>
-      </c>
-      <c r="D21" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7">
-        <v>99</v>
-      </c>
-      <c r="D22" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C23" s="7">
-        <v>1194</v>
+        <v>6236.25</v>
       </c>
       <c r="D23" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24" s="7">
-        <v>1322.22</v>
+        <v>2086</v>
       </c>
       <c r="D24" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C25" s="7">
-        <v>831.5</v>
+        <v>1194</v>
       </c>
       <c r="D25" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" s="7">
-        <v>24.99</v>
+        <v>99</v>
       </c>
       <c r="D26" s="7">
         <v>1</v>
@@ -1557,6 +1566,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState columnSort="1" ref="B18:D27">
+    <sortCondition ref="D18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit of calculated field fix. One failing test due to a sorting issue.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableWithCalculatedFields.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ems\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
   <si>
     <t>Transaction</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Nashville Total</t>
+  </si>
+  <si>
+    <t>Budgeted Total</t>
+  </si>
+  <si>
+    <t>Sum of CalculatedField3</t>
   </si>
 </sst>
 </file>
@@ -221,11 +227,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43479.658590509258" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43544.670320486111" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B2:H9" sheet="Sheet1"/>
+    <worksheetSource ref="B2:I9" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="11">
     <cacheField name="Transaction" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="20100007" maxValue="20100090"/>
     </cacheField>
@@ -252,12 +258,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Wholesale Price" numFmtId="8">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="415.75" count="4">
-        <n v="415.75"/>
-        <n v="99"/>
-        <n v="24.99"/>
-        <n v="199"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="415.75"/>
     </cacheField>
     <cacheField name="Units Sold" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="3">
@@ -269,7 +270,11 @@
     <cacheField name="Total" numFmtId="8">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="1194"/>
     </cacheField>
+    <cacheField name="Budgeted Total" numFmtId="8">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="20" maxValue="1500"/>
+    </cacheField>
     <cacheField name="CalculatedField" numFmtId="0" formula="'Wholesale Price'*'Units Sold'" databaseField="0"/>
+    <cacheField name="CalculatedField3" numFmtId="0" formula="Total/'Budgeted Total'" databaseField="0"/>
     <cacheField name="CalculatedField2" numFmtId="0" formula="CalculatedField/'Wholesale Price'" databaseField="0"/>
   </cacheFields>
   <extLst>
@@ -287,71 +292,162 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="415.75"/>
     <x v="0"/>
     <n v="415.75"/>
+    <n v="500"/>
   </r>
   <r>
     <n v="20100085"/>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="99"/>
     <x v="0"/>
     <n v="99"/>
+    <n v="100"/>
   </r>
   <r>
     <n v="20100083"/>
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="24.99"/>
     <x v="0"/>
     <n v="24.99"/>
+    <n v="20"/>
   </r>
   <r>
     <n v="20100007"/>
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="415.75"/>
     <x v="1"/>
     <n v="831.5"/>
+    <n v="755"/>
   </r>
   <r>
     <n v="20100070"/>
     <x v="2"/>
     <x v="1"/>
     <x v="3"/>
-    <x v="3"/>
+    <n v="199"/>
     <x v="2"/>
     <n v="1194"/>
+    <n v="1500"/>
   </r>
   <r>
     <n v="20100017"/>
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="415.75"/>
     <x v="1"/>
     <n v="831.5"/>
+    <n v="800"/>
   </r>
   <r>
     <n v="20100090"/>
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="415.75"/>
     <x v="1"/>
     <n v="831.5"/>
+    <n v="975"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B31:C42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of CalculatedField3" fld="9" baseField="0" baseItem="0" numFmtId="8"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G4:L14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="9">
+  <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="4">
@@ -388,7 +484,9 @@
       </items>
     </pivotField>
     <pivotField numFmtId="8" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
@@ -449,7 +547,7 @@
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of CalculatedField" fld="7" baseField="0" baseItem="0" numFmtId="8"/>
+    <dataField name="Sum of CalculatedField" fld="8" baseField="0" baseItem="0" numFmtId="8"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -460,10 +558,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B18:D27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+  <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -495,7 +593,9 @@
     <pivotField numFmtId="8" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField numFmtId="8" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
@@ -543,8 +643,8 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of CalculatedField" fld="7" baseField="0" baseItem="0" numFmtId="8"/>
-    <dataField name="Sum of CalculatedField2" fld="8" baseField="0" baseItem="0" numFmtId="8"/>
+    <dataField name="Sum of CalculatedField" fld="8" baseField="0" baseItem="0" numFmtId="8"/>
+    <dataField name="Sum of CalculatedField2" fld="10" baseField="0" baseItem="0" numFmtId="8"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -555,10 +655,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+  <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -568,14 +668,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="0"/>
@@ -585,18 +678,12 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField numFmtId="8" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField numFmtId="8" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
@@ -651,7 +738,7 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of CalculatedField" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of CalculatedField" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -925,16 +1012,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H9"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,8 +1049,11 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>20100076</v>
       </c>
@@ -979,8 +1075,11 @@
       <c r="H3" s="2">
         <v>415.75</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>20100085</v>
       </c>
@@ -1002,8 +1101,11 @@
       <c r="H4" s="2">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>20100083</v>
       </c>
@@ -1025,8 +1127,11 @@
       <c r="H5" s="2">
         <v>24.99</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>20100007</v>
       </c>
@@ -1048,8 +1153,11 @@
       <c r="H6" s="2">
         <v>831.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>20100070</v>
       </c>
@@ -1071,8 +1179,11 @@
       <c r="H7" s="2">
         <v>1194</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>20100017</v>
       </c>
@@ -1094,8 +1205,11 @@
       <c r="H8" s="2">
         <v>831.5</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>20100090</v>
       </c>
@@ -1116,6 +1230,9 @@
       </c>
       <c r="H9" s="2">
         <v>831.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -1125,17 +1242,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L27"/>
+  <dimension ref="B2:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
@@ -1565,6 +1682,102 @@
         <v>15</v>
       </c>
     </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.93217488789237668</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1.1013245033112582</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.85282051282051285</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.83150000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.80812499999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.79600000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1.0445</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1.2494999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1.0393749999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.90929892473118279</v>
+      </c>
+    </row>
   </sheetData>
   <sortState columnSort="1" ref="B18:D27">
     <sortCondition ref="D18"/>

</xml_diff>